<commit_message>
tests with 55 proportion
</commit_message>
<xml_diff>
--- a/Project/Files/results.xlsx
+++ b/Project/Files/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Classe</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>viver</t>
+  </si>
+  <si>
+    <t>55% - 600</t>
+  </si>
+  <si>
+    <t>55% - 1000</t>
   </si>
 </sst>
 </file>
@@ -180,12 +186,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -200,9 +224,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,250 +510,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.65</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>0.75</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.85</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
       <c r="B32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
       <c r="B34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>46</v>
       </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>